<commit_message>
can read and write data in excel
</commit_message>
<xml_diff>
--- a/ExcelValidate/ExcelData.xlsx
+++ b/ExcelValidate/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\source\repos\ExcelValidate\ExcelValidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D8E071-A236-4806-BD33-01FF89785C4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD10A9D-9AC3-4E9B-9DE3-D566DCED0352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
+    <workbookView xWindow="5616" yWindow="1992" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -96,9 +96,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D3A5CD-3859-4E63-9BBC-F3ADA0B7CE25}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,8 +462,73 @@
         <v>100000</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35920</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>1000.1</v>
+      </c>
+      <c r="E3">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2">
+        <v>35920</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1000.1</v>
+      </c>
+      <c r="E4">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="2">
+        <v>35920</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>1000.1</v>
+      </c>
+      <c r="E5">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>35920</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1000.1</v>
+      </c>
+      <c r="E6">
+        <v>100000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
valaditing column data for empty or null values as well as checking dateof birth column and Isactive column
</commit_message>
<xml_diff>
--- a/ExcelValidate/ExcelData.xlsx
+++ b/ExcelValidate/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\source\repos\ExcelValidate\ExcelValidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD10A9D-9AC3-4E9B-9DE3-D566DCED0352}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD78ABA-2A13-43A1-8EC0-5EE759348112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5616" yWindow="1992" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
+    <workbookView xWindow="3828" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Name</t>
   </si>
@@ -51,7 +51,7 @@
     <t>Rajesh</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>fdfsdfsdf</t>
   </si>
 </sst>
 </file>
@@ -416,7 +416,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="F6" sqref="F2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -452,8 +452,8 @@
       <c r="B2" s="2">
         <v>35920</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="C2" t="b">
+        <v>1</v>
       </c>
       <c r="D2">
         <v>1000.1</v>
@@ -469,8 +469,8 @@
       <c r="B3" s="2">
         <v>35920</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="C3" t="b">
+        <v>0</v>
       </c>
       <c r="D3">
         <v>1000.1</v>
@@ -483,11 +483,11 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2">
-        <v>35920</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="C4" t="b">
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1000.1</v>
@@ -500,8 +500,8 @@
       <c r="B5" s="2">
         <v>35920</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
+      <c r="C5" t="b">
+        <v>1</v>
       </c>
       <c r="D5">
         <v>1000.1</v>
@@ -517,8 +517,8 @@
       <c r="B6" s="2">
         <v>35920</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
+      <c r="C6" t="b">
+        <v>1</v>
       </c>
       <c r="D6">
         <v>1000.1</v>

</xml_diff>

<commit_message>
data validation working for all fields and api calls functioning as expected and added new newtonsoft package
</commit_message>
<xml_diff>
--- a/ExcelValidate/ExcelData.xlsx
+++ b/ExcelValidate/ExcelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\source\repos\ExcelValidate\ExcelValidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD78ABA-2A13-43A1-8EC0-5EE759348112}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56463274-DFA8-412C-8996-9EF7CE2C6A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3828" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
+    <workbookView xWindow="4824" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -51,14 +51,53 @@
     <t>Rajesh</t>
   </si>
   <si>
-    <t>fdfsdfsdf</t>
+    <t>Raj54esh</t>
+  </si>
+  <si>
+    <t>@Ra#je56sh</t>
+  </si>
+  <si>
+    <t>05-05-1998</t>
+  </si>
+  <si>
+    <t>sfds</t>
+  </si>
+  <si>
+    <t>dsdsd</t>
+  </si>
+  <si>
+    <t>$$$@!@</t>
+  </si>
+  <si>
+    <t>1000.11</t>
+  </si>
+  <si>
+    <t>fsdf</t>
+  </si>
+  <si>
+    <t>100$#000</t>
+  </si>
+  <si>
+    <t>2132Rajesh</t>
+  </si>
+  <si>
+    <t>qweqwd</t>
+  </si>
+  <si>
+    <t>15/11/2011</t>
+  </si>
+  <si>
+    <t>Prasad</t>
+  </si>
+  <si>
+    <t>aron</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +109,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,15 +139,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,35 +464,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D3A5CD-3859-4E63-9BBC-F3ADA0B7CE25}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F2:F6"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -449,28 +500,25 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="3">
         <v>35920</v>
       </c>
       <c r="C2" t="b">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>1000.1</v>
+        <v>1000.19</v>
       </c>
       <c r="E2">
-        <v>100000</v>
+        <v>3500</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="2">
-        <v>35920</v>
+      <c r="B3" s="3">
+        <v>35921</v>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>1000.1</v>
@@ -483,9 +531,6 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
-      </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
@@ -497,11 +542,11 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3">
         <v>35920</v>
-      </c>
-      <c r="C5" t="b">
-        <v>1</v>
       </c>
       <c r="D5">
         <v>1000.1</v>
@@ -514,21 +559,361 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="3">
+        <v>35921</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
         <v>35920</v>
       </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1000.1</v>
-      </c>
-      <c r="E6">
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1000.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>8523</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1000.1</v>
+      </c>
+      <c r="E8">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9">
+        <v>486.00150000000002</v>
+      </c>
+      <c r="C9" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>1000.1</v>
+      </c>
+      <c r="E9">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1000.1</v>
+      </c>
+      <c r="E10">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>1000.1</v>
+      </c>
+      <c r="E11">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1000.1896</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>35920</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1000.1</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1000.1</v>
+      </c>
+      <c r="E15">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="b">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1000.1</v>
+      </c>
+      <c r="E16">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" t="b">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>1000.1</v>
+      </c>
+      <c r="E17">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1000.1</v>
+      </c>
+      <c r="E18">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3">
+        <v>35921</v>
+      </c>
+      <c r="C19" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1000.1</v>
+      </c>
+      <c r="E19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43897</v>
+      </c>
+      <c r="C20">
+        <v>9875</v>
+      </c>
+      <c r="D20">
+        <v>1000.1</v>
+      </c>
+      <c r="E20">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C21" t="b">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>1000.1</v>
+      </c>
+      <c r="E21">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C22" t="b">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1000.1</v>
+      </c>
+      <c r="E22">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C23" t="b">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1000.1</v>
+      </c>
+      <c r="E23">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C24" t="b">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1000.1</v>
+      </c>
+      <c r="E24">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C25" t="b">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>1000.1</v>
+      </c>
+      <c r="E25">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>35920</v>
+      </c>
+      <c r="C26" t="b">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>1000.1</v>
+      </c>
+      <c r="E26">
         <v>100000</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <ignoredErrors>
+    <ignoredError sqref="D12" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaning up code and adding comments
</commit_message>
<xml_diff>
--- a/ExcelValidate/ExcelData.xlsx
+++ b/ExcelValidate/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\source\repos\ExcelValidate\ExcelValidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56463274-DFA8-412C-8996-9EF7CE2C6A8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A86A6D-0F9C-4A4B-91F0-9D52EC779934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4824" yWindow="828" windowWidth="17280" windowHeight="8964" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>aron</t>
+  </si>
+  <si>
+    <t>ApiStatus</t>
   </si>
 </sst>
 </file>
@@ -464,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D3A5CD-3859-4E63-9BBC-F3ADA0B7CE25}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,7 +482,7 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -495,8 +498,11 @@
       <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -513,7 +519,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B3" s="3">
         <v>35921</v>
       </c>
@@ -527,7 +533,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -541,7 +547,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -555,7 +561,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -569,7 +575,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -583,7 +589,7 @@
         <v>1000.1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -600,7 +606,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -617,7 +623,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -634,7 +640,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -651,7 +657,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -668,7 +674,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -685,7 +691,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -702,7 +708,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -719,7 +725,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Using better naming and refactoring for smaller codes
</commit_message>
<xml_diff>
--- a/ExcelValidate/ExcelData.xlsx
+++ b/ExcelValidate/ExcelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajesh\Desktop\Artelligence\ExcelValidate\ExcelValidate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F03BA87-8CE1-490B-9C12-E942D2261215}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8545413E-EAFD-48AB-9AEE-DA6BA48D26AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AE731715-8FC7-4097-8F2B-1F40C71D981B}"/>
   </bookViews>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F26"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>